<commit_message>
Jan 7 - Delete Derby and Add SQLite
</commit_message>
<xml_diff>
--- a/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/10poff.xlsx
+++ b/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/CrepeErase/10poff.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23627"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{F4CFDF92-07F1-4411-8B08-5F7982447492}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0B0E3354-4CC5-4F6A-8D1A-D59CAF88AD9F}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="8_{F4CFDF92-07F1-4411-8B08-5F7982447492}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{24698B84-73EF-4054-9C5A-EEA45D11548A}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="162">
   <si>
     <t>Vanity URL</t>
   </si>
@@ -239,6 +239,10 @@
   </si>
   <si>
     <t>Entry Promotion 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10% off entry price
+</t>
   </si>
   <si>
     <t>10% off entry price</t>
@@ -1209,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1671,7 +1675,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:5" s="34" customFormat="1" ht="15.75">
+    <row r="30" spans="1:5" s="34" customFormat="1" ht="31.5">
       <c r="A30" s="10" t="s">
         <v>70</v>
       </c>
@@ -1679,125 +1683,125 @@
         <v>71</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A31" s="10" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A32" s="10" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="11"/>
     </row>
     <row r="33" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A33" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="11" t="s">
-        <v>75</v>
-      </c>
       <c r="C33" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D33" s="11"/>
       <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A34" s="10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" s="34" customFormat="1" ht="330.75">
       <c r="A35" s="10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C35" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="11" t="s">
-        <v>79</v>
-      </c>
       <c r="E35" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A36" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A37" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A38" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B38" s="17">
         <v>59.95</v>
@@ -1814,7 +1818,7 @@
     </row>
     <row r="39" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A39" s="10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B39" s="12" t="s">
         <v>50</v>
@@ -1831,7 +1835,7 @@
     </row>
     <row r="40" spans="1:5" s="34" customFormat="1" ht="15.75" customHeight="1">
       <c r="A40" s="10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>53</v>
@@ -1848,7 +1852,7 @@
     </row>
     <row r="41" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A41" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B41" s="11">
         <v>3</v>
@@ -1865,69 +1869,69 @@
     </row>
     <row r="42" spans="1:5" s="34" customFormat="1" ht="31.5">
       <c r="A42" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C42" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>96</v>
-      </c>
       <c r="E42" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:5" s="34" customFormat="1" ht="157.5">
       <c r="A43" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C43" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="E43" s="13" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="34" customFormat="1" ht="141.75">
       <c r="A44" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D44" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E44" s="14" t="s">
         <v>104</v>
-      </c>
-      <c r="E44" s="14" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="45" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A45" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B45" s="11"/>
       <c r="C45" s="11" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D45" s="14"/>
       <c r="E45" s="14"/>
     </row>
     <row r="46" spans="1:5" ht="31.5">
       <c r="A46" s="32" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B46" s="35" t="s">
         <v>69</v>
@@ -1944,7 +1948,7 @@
     </row>
     <row r="47" spans="1:5" ht="15.75">
       <c r="A47" s="32" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B47" s="35"/>
       <c r="C47" s="35"/>
@@ -1953,7 +1957,7 @@
     </row>
     <row r="48" spans="1:5" ht="15.75">
       <c r="A48" s="32" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B48" s="33"/>
       <c r="C48" s="33"/>
@@ -1962,54 +1966,54 @@
     </row>
     <row r="49" spans="1:5" ht="15.75">
       <c r="A49" s="32" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B49" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C49" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D49" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E49" s="35" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75">
       <c r="A50" s="32" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B50" s="33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C50" s="33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D50" s="33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E50" s="33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75">
       <c r="A51" s="32" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B51" s="33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C51" s="33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D51" s="36"/>
       <c r="E51" s="36"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="A52" s="32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B52" s="33">
         <v>5</v>
@@ -2026,41 +2030,41 @@
     </row>
     <row r="53" spans="1:5" ht="15.75">
       <c r="A53" s="32" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B53" s="33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C53" s="33" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D53" s="33" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E53" s="33" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75">
       <c r="A54" s="32" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B54" s="33" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C54" s="33" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D54" s="33" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E54" s="33" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75">
       <c r="A55" s="32" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B55" s="33">
         <v>3</v>
@@ -2077,30 +2081,30 @@
     </row>
     <row r="56" spans="1:5" ht="15.75">
       <c r="A56" s="32" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B56" s="33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C56" s="33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D56" s="33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E56" s="33" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A57" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D57" s="17">
         <v>59.95</v>
@@ -2111,13 +2115,13 @@
     </row>
     <row r="58" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A58" s="10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D58" s="17">
         <v>3.99</v>
@@ -2128,24 +2132,24 @@
     </row>
     <row r="59" spans="1:5" s="34" customFormat="1" ht="15.75">
       <c r="A59" s="10" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E59" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75">
       <c r="A60" s="32" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B60" s="33">
         <v>3</v>
@@ -2162,7 +2166,7 @@
     </row>
     <row r="61" spans="1:5" s="8" customFormat="1" ht="15.75">
       <c r="A61" s="40" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B61" s="41"/>
       <c r="C61" s="41"/>
@@ -2171,7 +2175,7 @@
     </row>
     <row r="62" spans="1:5" ht="15.75">
       <c r="A62" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -2180,7 +2184,7 @@
     </row>
     <row r="63" spans="1:5" ht="15.75">
       <c r="A63" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -2189,7 +2193,7 @@
     </row>
     <row r="64" spans="1:5" ht="15.75">
       <c r="A64" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B64" s="3"/>
       <c r="C64" s="4"/>
@@ -2198,7 +2202,7 @@
     </row>
     <row r="65" spans="1:5" ht="15.75">
       <c r="A65" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -2207,7 +2211,7 @@
     </row>
     <row r="66" spans="1:5" ht="15.75">
       <c r="A66" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -2216,7 +2220,7 @@
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1">
       <c r="A67" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -2225,7 +2229,7 @@
     </row>
     <row r="68" spans="1:5" ht="15.75">
       <c r="A68" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -2234,7 +2238,7 @@
     </row>
     <row r="69" spans="1:5" ht="15.75">
       <c r="A69" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -2243,7 +2247,7 @@
     </row>
     <row r="70" spans="1:5" ht="15.75">
       <c r="A70" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -2252,7 +2256,7 @@
     </row>
     <row r="71" spans="1:5" ht="15.75">
       <c r="A71" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -2261,7 +2265,7 @@
     </row>
     <row r="72" spans="1:5" ht="15.75">
       <c r="A72" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -2270,7 +2274,7 @@
     </row>
     <row r="73" spans="1:5" ht="15.75">
       <c r="A73" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -2279,7 +2283,7 @@
     </row>
     <row r="74" spans="1:5" ht="15.75">
       <c r="A74" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -2288,7 +2292,7 @@
     </row>
     <row r="75" spans="1:5" ht="15.75">
       <c r="A75" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -2297,7 +2301,7 @@
     </row>
     <row r="76" spans="1:5" ht="15.75">
       <c r="A76" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -2306,7 +2310,7 @@
     </row>
     <row r="77" spans="1:5" ht="15.75">
       <c r="A77" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -2315,7 +2319,7 @@
     </row>
     <row r="78" spans="1:5" ht="15.75">
       <c r="A78" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -2324,7 +2328,7 @@
     </row>
     <row r="79" spans="1:5" ht="15.75">
       <c r="A79" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -2333,7 +2337,7 @@
     </row>
     <row r="80" spans="1:5" ht="31.5">
       <c r="A80" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -2342,7 +2346,7 @@
     </row>
     <row r="81" spans="1:5" ht="15.75">
       <c r="A81" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -2351,7 +2355,7 @@
     </row>
     <row r="82" spans="1:5" ht="15.75">
       <c r="A82" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -2360,7 +2364,7 @@
     </row>
     <row r="83" spans="1:5" ht="15.75">
       <c r="A83" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -2369,7 +2373,7 @@
     </row>
     <row r="84" spans="1:5" ht="15.75">
       <c r="A84" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -2378,7 +2382,7 @@
     </row>
     <row r="85" spans="1:5" ht="15.75">
       <c r="A85" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -2387,7 +2391,7 @@
     </row>
     <row r="86" spans="1:5" ht="15.75">
       <c r="A86" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -2396,7 +2400,7 @@
     </row>
     <row r="87" spans="1:5" ht="15.75">
       <c r="A87" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -2405,7 +2409,7 @@
     </row>
     <row r="88" spans="1:5" ht="31.5">
       <c r="A88" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -2414,7 +2418,7 @@
     </row>
     <row r="89" spans="1:5" ht="15.75">
       <c r="A89" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -2423,7 +2427,7 @@
     </row>
     <row r="90" spans="1:5" ht="31.5">
       <c r="A90" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -2432,7 +2436,7 @@
     </row>
     <row r="91" spans="1:5" ht="15.75">
       <c r="A91" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -2441,7 +2445,7 @@
     </row>
     <row r="92" spans="1:5" ht="31.5">
       <c r="A92" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -2450,7 +2454,7 @@
     </row>
     <row r="93" spans="1:5" ht="15.75">
       <c r="A93" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -2459,7 +2463,7 @@
     </row>
     <row r="94" spans="1:5" ht="15.75">
       <c r="A94" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -2468,7 +2472,7 @@
     </row>
     <row r="95" spans="1:5" ht="15.75">
       <c r="A95" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -2477,7 +2481,7 @@
     </row>
     <row r="96" spans="1:5" ht="15.75">
       <c r="A96" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -2486,7 +2490,7 @@
     </row>
     <row r="97" spans="1:5" ht="15.75">
       <c r="A97" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -2495,7 +2499,7 @@
     </row>
     <row r="98" spans="1:5" ht="15.75">
       <c r="A98" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -2504,7 +2508,7 @@
     </row>
     <row r="99" spans="1:5" ht="15.75">
       <c r="A99" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -2513,7 +2517,7 @@
     </row>
     <row r="100" spans="1:5" ht="15.75">
       <c r="A100" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -2522,7 +2526,7 @@
     </row>
     <row r="101" spans="1:5" ht="15.75">
       <c r="A101" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -2531,7 +2535,7 @@
     </row>
     <row r="102" spans="1:5" ht="15.75">
       <c r="A102" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -2540,7 +2544,7 @@
     </row>
     <row r="103" spans="1:5" ht="15.75">
       <c r="A103" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
@@ -2549,7 +2553,7 @@
     </row>
     <row r="104" spans="1:5" ht="15.75">
       <c r="A104" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
@@ -2558,7 +2562,7 @@
     </row>
     <row r="105" spans="1:5" ht="15.75">
       <c r="A105" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -2567,7 +2571,7 @@
     </row>
     <row r="106" spans="1:5" ht="15.75">
       <c r="A106" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -2576,7 +2580,7 @@
     </row>
     <row r="107" spans="1:5" ht="15.75">
       <c r="A107" s="6" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B107" s="8"/>
       <c r="C107" s="8"/>
@@ -2597,15 +2601,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C47EEB8100460B478BDC3BCCBE3D5051" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="829e995fc61fbfa25718206016b29da6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2" xmlns:ns3="3e63a3be-2d53-41f2-914e-dd0efc332534" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3545440ad2b936a9d10385f8b267d779" ns2:_="" ns3:_="">
     <xsd:import namespace="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2"/>
@@ -2770,6 +2765,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2777,11 +2781,11 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE300D08-B0CB-4DA8-9AA7-F031ED0BA7B6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59656202-A0B0-43EC-AE8C-F4D1B807D10E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{59656202-A0B0-43EC-AE8C-F4D1B807D10E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE300D08-B0CB-4DA8-9AA7-F031ED0BA7B6}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>